<commit_message>
Edição dos nomes de editais anteriores
</commit_message>
<xml_diff>
--- a/501pra_manha.xlsx
+++ b/501pra_manha.xlsx
@@ -22,45 +22,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">MICHELE CRISTIANE DE MORAES ECASTRO DUTRA Edital 01/2021 (item 9.14.1 do
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Edital 501)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>BÁRBARA ALVIM MARQUES SIMAS (item 9.14.1 do Edital 501)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>MONICA MARIA RODRIGUES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t>MARIA APARECIDA DA SILVA</t>
     </r>
   </si>
@@ -1432,6 +1393,25 @@
         <family val="1"/>
       </rPr>
       <t>JUSSARA APARECIDA DA SILVA</t>
+    </r>
+  </si>
+  <si>
+    <t>MONICA MARIA RODRIGUES</t>
+  </si>
+  <si>
+    <t>BÁRBARA ALVIM MARQUES SIMAS (9.14.1)</t>
+  </si>
+  <si>
+    <r>
+      <t>MICHELE CRISTIANE DE MORAES ECASTRO DUTRA  (9.14.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
     </r>
   </si>
 </sst>
@@ -1538,10 +1518,10 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1854,7 +1834,7 @@
   <dimension ref="A1:B272"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1868,8 +1848,8 @@
       <c r="A1" s="2">
         <v>980</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
+      <c r="B1" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
@@ -1877,7 +1857,7 @@
         <v>2508</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="31.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -1885,1119 +1865,1119 @@
         <v>2235</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>2</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2236</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>3</v>
+      <c r="B4" s="3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2237</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>2238</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>5</v>
+      <c r="B6" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2239</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>6</v>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2240</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>7</v>
+      <c r="B8" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2241</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>8</v>
+      <c r="B9" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2242</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>9</v>
+      <c r="B10" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>2243</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>10</v>
+      <c r="B11" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>2244</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>11</v>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>2245</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>12</v>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>2246</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>13</v>
+      <c r="B14" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>2247</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>14</v>
+      <c r="B15" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>2248</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>15</v>
+      <c r="B16" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>2249</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>16</v>
+      <c r="B17" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>2250</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>17</v>
+      <c r="B18" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>2251</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>18</v>
+      <c r="B19" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>2252</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>19</v>
+      <c r="B20" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>2253</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>20</v>
+      <c r="B21" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>2254</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>21</v>
+      <c r="B22" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>2255</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>22</v>
+      <c r="B23" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>2256</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>23</v>
+      <c r="B24" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>2257</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>24</v>
+      <c r="B25" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>2258</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>25</v>
+      <c r="B26" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>2259</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>26</v>
+      <c r="B27" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>2260</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>27</v>
+      <c r="B28" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>2261</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>28</v>
+      <c r="B29" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>2262</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>29</v>
+      <c r="B30" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>2263</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>30</v>
+      <c r="B31" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>2264</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>31</v>
+      <c r="B32" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>2265</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>32</v>
+      <c r="B33" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>2266</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>33</v>
+      <c r="B34" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>2267</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>34</v>
+      <c r="B35" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>2268</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>35</v>
+      <c r="B36" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>2269</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>36</v>
+      <c r="B37" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>2270</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>37</v>
+      <c r="B38" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>2271</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>38</v>
+      <c r="B39" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>2272</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>39</v>
+      <c r="B40" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>2273</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>40</v>
+      <c r="B41" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>2274</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>41</v>
+      <c r="B42" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>2275</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>42</v>
+      <c r="B43" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>2276</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>43</v>
+      <c r="B44" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>2277</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>44</v>
+      <c r="B45" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>2278</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>45</v>
+      <c r="B46" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>2279</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>46</v>
+      <c r="B47" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>2280</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>47</v>
+      <c r="B48" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>2281</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>48</v>
+      <c r="B49" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>2282</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>49</v>
+      <c r="B50" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>2283</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>50</v>
+      <c r="B51" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>2284</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>51</v>
+      <c r="B52" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>2285</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>52</v>
+      <c r="B53" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>2286</v>
       </c>
-      <c r="B54" s="4" t="s">
-        <v>53</v>
+      <c r="B54" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>2287</v>
       </c>
-      <c r="B55" s="4" t="s">
-        <v>54</v>
+      <c r="B55" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>2288</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>55</v>
+      <c r="B56" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>2289</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>56</v>
+      <c r="B57" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>2290</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>57</v>
+      <c r="B58" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>2291</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>58</v>
+      <c r="B59" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>2292</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>59</v>
+      <c r="B60" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>2293</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>60</v>
+      <c r="B61" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>2294</v>
       </c>
-      <c r="B62" s="4" t="s">
-        <v>61</v>
+      <c r="B62" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>2295</v>
       </c>
-      <c r="B63" s="4" t="s">
-        <v>62</v>
+      <c r="B63" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>2296</v>
       </c>
-      <c r="B64" s="4" t="s">
-        <v>63</v>
+      <c r="B64" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>2297</v>
       </c>
-      <c r="B65" s="4" t="s">
-        <v>64</v>
+      <c r="B65" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>2298</v>
       </c>
-      <c r="B66" s="4" t="s">
-        <v>65</v>
+      <c r="B66" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>2299</v>
       </c>
-      <c r="B67" s="4" t="s">
-        <v>66</v>
+      <c r="B67" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>2300</v>
       </c>
-      <c r="B68" s="4" t="s">
-        <v>67</v>
+      <c r="B68" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>2301</v>
       </c>
-      <c r="B69" s="4" t="s">
-        <v>68</v>
+      <c r="B69" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>2302</v>
       </c>
-      <c r="B70" s="4" t="s">
-        <v>69</v>
+      <c r="B70" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>2303</v>
       </c>
-      <c r="B71" s="4" t="s">
-        <v>70</v>
+      <c r="B71" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>2304</v>
       </c>
-      <c r="B72" s="4" t="s">
-        <v>71</v>
+      <c r="B72" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>2305</v>
       </c>
-      <c r="B73" s="4" t="s">
-        <v>72</v>
+      <c r="B73" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>2306</v>
       </c>
-      <c r="B74" s="4" t="s">
-        <v>73</v>
+      <c r="B74" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>2307</v>
       </c>
-      <c r="B75" s="4" t="s">
-        <v>74</v>
+      <c r="B75" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>2308</v>
       </c>
-      <c r="B76" s="4" t="s">
-        <v>75</v>
+      <c r="B76" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>2309</v>
       </c>
-      <c r="B77" s="4" t="s">
-        <v>76</v>
+      <c r="B77" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>2310</v>
       </c>
-      <c r="B78" s="4" t="s">
-        <v>77</v>
+      <c r="B78" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>2311</v>
       </c>
-      <c r="B79" s="4" t="s">
-        <v>78</v>
+      <c r="B79" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>2312</v>
       </c>
-      <c r="B80" s="4" t="s">
-        <v>79</v>
+      <c r="B80" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>2313</v>
       </c>
-      <c r="B81" s="4" t="s">
-        <v>80</v>
+      <c r="B81" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>2314</v>
       </c>
-      <c r="B82" s="4" t="s">
-        <v>81</v>
+      <c r="B82" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>2315</v>
       </c>
-      <c r="B83" s="4" t="s">
-        <v>82</v>
+      <c r="B83" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>2316</v>
       </c>
-      <c r="B84" s="4" t="s">
-        <v>83</v>
+      <c r="B84" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>2317</v>
       </c>
-      <c r="B85" s="4" t="s">
-        <v>84</v>
+      <c r="B85" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>2318</v>
       </c>
-      <c r="B86" s="4" t="s">
-        <v>85</v>
+      <c r="B86" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>2319</v>
       </c>
-      <c r="B87" s="4" t="s">
-        <v>86</v>
+      <c r="B87" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>2320</v>
       </c>
-      <c r="B88" s="4" t="s">
-        <v>87</v>
+      <c r="B88" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>2321</v>
       </c>
-      <c r="B89" s="4" t="s">
-        <v>88</v>
+      <c r="B89" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>2322</v>
       </c>
-      <c r="B90" s="4" t="s">
-        <v>89</v>
+      <c r="B90" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>2323</v>
       </c>
-      <c r="B91" s="4" t="s">
-        <v>90</v>
+      <c r="B91" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>2324</v>
       </c>
-      <c r="B92" s="4" t="s">
-        <v>91</v>
+      <c r="B92" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>2325</v>
       </c>
-      <c r="B93" s="4" t="s">
-        <v>92</v>
+      <c r="B93" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>2326</v>
       </c>
-      <c r="B94" s="4" t="s">
-        <v>93</v>
+      <c r="B94" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>2327</v>
       </c>
-      <c r="B95" s="4" t="s">
-        <v>94</v>
+      <c r="B95" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>2328</v>
       </c>
-      <c r="B96" s="4" t="s">
-        <v>95</v>
+      <c r="B96" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>2329</v>
       </c>
-      <c r="B97" s="4" t="s">
-        <v>96</v>
+      <c r="B97" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>2330</v>
       </c>
-      <c r="B98" s="4" t="s">
-        <v>97</v>
+      <c r="B98" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>2331</v>
       </c>
-      <c r="B99" s="4" t="s">
-        <v>98</v>
+      <c r="B99" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>2332</v>
       </c>
-      <c r="B100" s="4" t="s">
-        <v>99</v>
+      <c r="B100" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>2333</v>
       </c>
-      <c r="B101" s="4" t="s">
-        <v>100</v>
+      <c r="B101" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>2334</v>
       </c>
-      <c r="B102" s="4" t="s">
-        <v>101</v>
+      <c r="B102" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>2335</v>
       </c>
-      <c r="B103" s="4" t="s">
-        <v>102</v>
+      <c r="B103" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>2336</v>
       </c>
-      <c r="B104" s="4" t="s">
-        <v>103</v>
+      <c r="B104" s="3" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>2337</v>
       </c>
-      <c r="B105" s="4" t="s">
-        <v>104</v>
+      <c r="B105" s="3" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>2338</v>
       </c>
-      <c r="B106" s="4" t="s">
-        <v>105</v>
+      <c r="B106" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>2339</v>
       </c>
-      <c r="B107" s="4" t="s">
-        <v>106</v>
+      <c r="B107" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>2340</v>
       </c>
-      <c r="B108" s="4" t="s">
-        <v>107</v>
+      <c r="B108" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>2341</v>
       </c>
-      <c r="B109" s="4" t="s">
-        <v>108</v>
+      <c r="B109" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>2342</v>
       </c>
-      <c r="B110" s="4" t="s">
-        <v>109</v>
+      <c r="B110" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>2343</v>
       </c>
-      <c r="B111" s="4" t="s">
-        <v>110</v>
+      <c r="B111" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>2344</v>
       </c>
-      <c r="B112" s="4" t="s">
-        <v>111</v>
+      <c r="B112" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>2345</v>
       </c>
-      <c r="B113" s="4" t="s">
-        <v>112</v>
+      <c r="B113" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>2346</v>
       </c>
-      <c r="B114" s="4" t="s">
-        <v>113</v>
+      <c r="B114" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>2347</v>
       </c>
-      <c r="B115" s="4" t="s">
-        <v>114</v>
+      <c r="B115" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>2348</v>
       </c>
-      <c r="B116" s="4" t="s">
-        <v>115</v>
+      <c r="B116" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>2349</v>
       </c>
-      <c r="B117" s="4" t="s">
-        <v>116</v>
+      <c r="B117" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>2350</v>
       </c>
-      <c r="B118" s="4" t="s">
-        <v>32</v>
+      <c r="B118" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>2351</v>
       </c>
-      <c r="B119" s="4" t="s">
-        <v>117</v>
+      <c r="B119" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>2352</v>
       </c>
-      <c r="B120" s="4" t="s">
-        <v>118</v>
+      <c r="B120" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>2353</v>
       </c>
-      <c r="B121" s="4" t="s">
-        <v>119</v>
+      <c r="B121" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>2354</v>
       </c>
-      <c r="B122" s="4" t="s">
-        <v>120</v>
+      <c r="B122" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>2355</v>
       </c>
-      <c r="B123" s="4" t="s">
-        <v>121</v>
+      <c r="B123" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>2356</v>
       </c>
-      <c r="B124" s="4" t="s">
-        <v>122</v>
+      <c r="B124" s="3" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>2357</v>
       </c>
-      <c r="B125" s="4" t="s">
-        <v>123</v>
+      <c r="B125" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>2358</v>
       </c>
-      <c r="B126" s="4" t="s">
-        <v>124</v>
+      <c r="B126" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>2359</v>
       </c>
-      <c r="B127" s="4" t="s">
-        <v>125</v>
+      <c r="B127" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>2360</v>
       </c>
-      <c r="B128" s="4" t="s">
-        <v>126</v>
+      <c r="B128" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>2361</v>
       </c>
-      <c r="B129" s="4" t="s">
-        <v>127</v>
+      <c r="B129" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>2362</v>
       </c>
-      <c r="B130" s="4" t="s">
-        <v>128</v>
+      <c r="B130" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>2363</v>
       </c>
-      <c r="B131" s="4" t="s">
-        <v>129</v>
+      <c r="B131" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>2364</v>
       </c>
-      <c r="B132" s="4" t="s">
-        <v>130</v>
+      <c r="B132" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>2365</v>
       </c>
-      <c r="B133" s="4" t="s">
-        <v>131</v>
+      <c r="B133" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>2366</v>
       </c>
-      <c r="B134" s="4" t="s">
-        <v>132</v>
+      <c r="B134" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
         <v>2367</v>
       </c>
-      <c r="B135" s="4" t="s">
-        <v>133</v>
+      <c r="B135" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>2368</v>
       </c>
-      <c r="B136" s="4" t="s">
-        <v>134</v>
+      <c r="B136" s="3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
         <v>2369</v>
       </c>
-      <c r="B137" s="4" t="s">
-        <v>135</v>
+      <c r="B137" s="3" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>2370</v>
       </c>
-      <c r="B138" s="4" t="s">
-        <v>136</v>
+      <c r="B138" s="3" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
         <v>2371</v>
       </c>
-      <c r="B139" s="4" t="s">
-        <v>137</v>
+      <c r="B139" s="3" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>2372</v>
       </c>
-      <c r="B140" s="4" t="s">
-        <v>138</v>
+      <c r="B140" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
         <v>2373</v>
       </c>
-      <c r="B141" s="4" t="s">
-        <v>139</v>
+      <c r="B141" s="3" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
         <v>2374</v>
       </c>
-      <c r="B142" s="4" t="s">
-        <v>140</v>
+      <c r="B142" s="3" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
@@ -3018,83 +2998,83 @@
     </row>
     <row r="147" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="2"/>
-      <c r="B147" s="4"/>
+      <c r="B147" s="3"/>
     </row>
     <row r="148" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="2"/>
-      <c r="B148" s="4"/>
+      <c r="B148" s="3"/>
     </row>
     <row r="149" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="2"/>
-      <c r="B149" s="4"/>
+      <c r="B149" s="3"/>
     </row>
     <row r="150" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="2"/>
-      <c r="B150" s="4"/>
+      <c r="B150" s="3"/>
     </row>
     <row r="151" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="2"/>
-      <c r="B151" s="4"/>
+      <c r="B151" s="3"/>
     </row>
     <row r="152" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="2"/>
-      <c r="B152" s="4"/>
+      <c r="B152" s="3"/>
     </row>
     <row r="153" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="2"/>
-      <c r="B153" s="4"/>
+      <c r="B153" s="3"/>
     </row>
     <row r="154" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="2"/>
-      <c r="B154" s="4"/>
+      <c r="B154" s="3"/>
     </row>
     <row r="155" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="2"/>
-      <c r="B155" s="4"/>
+      <c r="B155" s="3"/>
     </row>
     <row r="156" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="2"/>
-      <c r="B156" s="4"/>
+      <c r="B156" s="3"/>
     </row>
     <row r="157" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="2"/>
-      <c r="B157" s="4"/>
+      <c r="B157" s="3"/>
     </row>
     <row r="158" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="2"/>
-      <c r="B158" s="4"/>
+      <c r="B158" s="3"/>
     </row>
     <row r="159" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="2"/>
-      <c r="B159" s="4"/>
+      <c r="B159" s="3"/>
     </row>
     <row r="160" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="2"/>
-      <c r="B160" s="4"/>
+      <c r="B160" s="3"/>
     </row>
     <row r="161" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="2"/>
-      <c r="B161" s="4"/>
+      <c r="B161" s="3"/>
     </row>
     <row r="162" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="2"/>
-      <c r="B162" s="4"/>
+      <c r="B162" s="3"/>
     </row>
     <row r="163" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="2"/>
-      <c r="B163" s="4"/>
+      <c r="B163" s="3"/>
     </row>
     <row r="164" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="2"/>
-      <c r="B164" s="4"/>
+      <c r="B164" s="3"/>
     </row>
     <row r="165" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="2"/>
-      <c r="B165" s="4"/>
+      <c r="B165" s="3"/>
     </row>
     <row r="166" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="2"/>
-      <c r="B166" s="4"/>
+      <c r="B166" s="3"/>
     </row>
     <row r="167" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="5"/>
@@ -3106,411 +3086,411 @@
     </row>
     <row r="169" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="2"/>
-      <c r="B169" s="4"/>
+      <c r="B169" s="3"/>
     </row>
     <row r="170" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="2"/>
-      <c r="B170" s="4"/>
+      <c r="B170" s="3"/>
     </row>
     <row r="171" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="2"/>
-      <c r="B171" s="4"/>
+      <c r="B171" s="3"/>
     </row>
     <row r="172" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="2"/>
-      <c r="B172" s="4"/>
+      <c r="B172" s="3"/>
     </row>
     <row r="173" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="2"/>
-      <c r="B173" s="4"/>
+      <c r="B173" s="3"/>
     </row>
     <row r="174" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="2"/>
-      <c r="B174" s="4"/>
+      <c r="B174" s="3"/>
     </row>
     <row r="175" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="2"/>
-      <c r="B175" s="4"/>
+      <c r="B175" s="3"/>
     </row>
     <row r="176" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="2"/>
-      <c r="B176" s="4"/>
+      <c r="B176" s="3"/>
     </row>
     <row r="177" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="2"/>
-      <c r="B177" s="4"/>
+      <c r="B177" s="3"/>
     </row>
     <row r="178" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="2"/>
-      <c r="B178" s="4"/>
+      <c r="B178" s="3"/>
     </row>
     <row r="179" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="2"/>
-      <c r="B179" s="4"/>
+      <c r="B179" s="3"/>
     </row>
     <row r="180" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="2"/>
-      <c r="B180" s="4"/>
+      <c r="B180" s="3"/>
     </row>
     <row r="181" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="2"/>
-      <c r="B181" s="4"/>
+      <c r="B181" s="3"/>
     </row>
     <row r="182" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="2"/>
-      <c r="B182" s="4"/>
+      <c r="B182" s="3"/>
     </row>
     <row r="183" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="2"/>
-      <c r="B183" s="4"/>
+      <c r="B183" s="3"/>
     </row>
     <row r="184" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="2"/>
-      <c r="B184" s="4"/>
+      <c r="B184" s="3"/>
     </row>
     <row r="185" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="2"/>
-      <c r="B185" s="4"/>
+      <c r="B185" s="3"/>
     </row>
     <row r="186" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="2"/>
-      <c r="B186" s="4"/>
+      <c r="B186" s="3"/>
     </row>
     <row r="187" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="2"/>
-      <c r="B187" s="4"/>
+      <c r="B187" s="3"/>
     </row>
     <row r="188" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="2"/>
-      <c r="B188" s="4"/>
+      <c r="B188" s="3"/>
     </row>
     <row r="189" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="2"/>
-      <c r="B189" s="4"/>
+      <c r="B189" s="3"/>
     </row>
     <row r="190" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="2"/>
-      <c r="B190" s="4"/>
+      <c r="B190" s="3"/>
     </row>
     <row r="191" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="2"/>
-      <c r="B191" s="4"/>
+      <c r="B191" s="3"/>
     </row>
     <row r="192" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="2"/>
-      <c r="B192" s="4"/>
+      <c r="B192" s="3"/>
     </row>
     <row r="193" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="2"/>
-      <c r="B193" s="4"/>
+      <c r="B193" s="3"/>
     </row>
     <row r="194" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="2"/>
-      <c r="B194" s="4"/>
+      <c r="B194" s="3"/>
     </row>
     <row r="195" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="2"/>
-      <c r="B195" s="4"/>
+      <c r="B195" s="3"/>
     </row>
     <row r="196" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="2"/>
-      <c r="B196" s="4"/>
+      <c r="B196" s="3"/>
     </row>
     <row r="197" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="2"/>
-      <c r="B197" s="4"/>
+      <c r="B197" s="3"/>
     </row>
     <row r="198" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="2"/>
-      <c r="B198" s="4"/>
+      <c r="B198" s="3"/>
     </row>
     <row r="199" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="2"/>
-      <c r="B199" s="4"/>
+      <c r="B199" s="3"/>
     </row>
     <row r="200" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="2"/>
-      <c r="B200" s="4"/>
+      <c r="B200" s="3"/>
     </row>
     <row r="201" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="2"/>
-      <c r="B201" s="4"/>
+      <c r="B201" s="3"/>
     </row>
     <row r="202" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="2"/>
-      <c r="B202" s="4"/>
+      <c r="B202" s="3"/>
     </row>
     <row r="203" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="2"/>
-      <c r="B203" s="4"/>
+      <c r="B203" s="3"/>
     </row>
     <row r="204" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="2"/>
-      <c r="B204" s="4"/>
+      <c r="B204" s="3"/>
     </row>
     <row r="205" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="2"/>
-      <c r="B205" s="4"/>
+      <c r="B205" s="3"/>
     </row>
     <row r="206" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="2"/>
-      <c r="B206" s="4"/>
+      <c r="B206" s="3"/>
     </row>
     <row r="207" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="2"/>
-      <c r="B207" s="4"/>
+      <c r="B207" s="3"/>
     </row>
     <row r="208" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="2"/>
-      <c r="B208" s="4"/>
+      <c r="B208" s="3"/>
     </row>
     <row r="209" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="2"/>
-      <c r="B209" s="4"/>
+      <c r="B209" s="3"/>
     </row>
     <row r="210" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="2"/>
-      <c r="B210" s="4"/>
+      <c r="B210" s="3"/>
     </row>
     <row r="211" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="2"/>
-      <c r="B211" s="4"/>
+      <c r="B211" s="3"/>
     </row>
     <row r="212" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="2"/>
-      <c r="B212" s="4"/>
+      <c r="B212" s="3"/>
     </row>
     <row r="213" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="2"/>
-      <c r="B213" s="4"/>
+      <c r="B213" s="3"/>
     </row>
     <row r="214" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="2"/>
-      <c r="B214" s="4"/>
+      <c r="B214" s="3"/>
     </row>
     <row r="215" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="2"/>
-      <c r="B215" s="4"/>
+      <c r="B215" s="3"/>
     </row>
     <row r="216" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="2"/>
-      <c r="B216" s="4"/>
+      <c r="B216" s="3"/>
     </row>
     <row r="217" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="2"/>
-      <c r="B217" s="4"/>
+      <c r="B217" s="3"/>
     </row>
     <row r="218" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="2"/>
-      <c r="B218" s="4"/>
+      <c r="B218" s="3"/>
     </row>
     <row r="219" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="2"/>
-      <c r="B219" s="4"/>
+      <c r="B219" s="3"/>
     </row>
     <row r="220" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="2"/>
-      <c r="B220" s="4"/>
+      <c r="B220" s="3"/>
     </row>
     <row r="221" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="2"/>
-      <c r="B221" s="4"/>
+      <c r="B221" s="3"/>
     </row>
     <row r="222" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="2"/>
-      <c r="B222" s="4"/>
+      <c r="B222" s="3"/>
     </row>
     <row r="223" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="2"/>
-      <c r="B223" s="4"/>
+      <c r="B223" s="3"/>
     </row>
     <row r="224" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="2"/>
-      <c r="B224" s="4"/>
+      <c r="B224" s="3"/>
     </row>
     <row r="225" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="2"/>
-      <c r="B225" s="4"/>
+      <c r="B225" s="3"/>
     </row>
     <row r="226" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="2"/>
-      <c r="B226" s="4"/>
+      <c r="B226" s="3"/>
     </row>
     <row r="227" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="2"/>
-      <c r="B227" s="4"/>
+      <c r="B227" s="3"/>
     </row>
     <row r="228" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="2"/>
-      <c r="B228" s="4"/>
+      <c r="B228" s="3"/>
     </row>
     <row r="229" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="2"/>
-      <c r="B229" s="4"/>
+      <c r="B229" s="3"/>
     </row>
     <row r="230" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="2"/>
-      <c r="B230" s="4"/>
+      <c r="B230" s="3"/>
     </row>
     <row r="231" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="2"/>
-      <c r="B231" s="4"/>
+      <c r="B231" s="3"/>
     </row>
     <row r="232" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="2"/>
-      <c r="B232" s="4"/>
+      <c r="B232" s="3"/>
     </row>
     <row r="233" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="2"/>
-      <c r="B233" s="4"/>
+      <c r="B233" s="3"/>
     </row>
     <row r="234" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="2"/>
-      <c r="B234" s="4"/>
+      <c r="B234" s="3"/>
     </row>
     <row r="235" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="2"/>
-      <c r="B235" s="4"/>
+      <c r="B235" s="3"/>
     </row>
     <row r="236" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="2"/>
-      <c r="B236" s="4"/>
+      <c r="B236" s="3"/>
     </row>
     <row r="237" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="2"/>
-      <c r="B237" s="4"/>
+      <c r="B237" s="3"/>
     </row>
     <row r="238" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="2"/>
-      <c r="B238" s="4"/>
+      <c r="B238" s="3"/>
     </row>
     <row r="239" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="2"/>
-      <c r="B239" s="4"/>
+      <c r="B239" s="3"/>
     </row>
     <row r="240" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="2"/>
-      <c r="B240" s="4"/>
+      <c r="B240" s="3"/>
     </row>
     <row r="241" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="2"/>
-      <c r="B241" s="4"/>
+      <c r="B241" s="3"/>
     </row>
     <row r="242" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="2"/>
-      <c r="B242" s="4"/>
+      <c r="B242" s="3"/>
     </row>
     <row r="243" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="2"/>
-      <c r="B243" s="4"/>
+      <c r="B243" s="3"/>
     </row>
     <row r="244" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="2"/>
-      <c r="B244" s="4"/>
+      <c r="B244" s="3"/>
     </row>
     <row r="245" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="2"/>
-      <c r="B245" s="4"/>
+      <c r="B245" s="3"/>
     </row>
     <row r="246" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="2"/>
-      <c r="B246" s="4"/>
+      <c r="B246" s="3"/>
     </row>
     <row r="247" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="2"/>
-      <c r="B247" s="4"/>
+      <c r="B247" s="3"/>
     </row>
     <row r="248" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="2"/>
-      <c r="B248" s="4"/>
+      <c r="B248" s="3"/>
     </row>
     <row r="249" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="2"/>
-      <c r="B249" s="4"/>
+      <c r="B249" s="3"/>
     </row>
     <row r="250" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="2"/>
-      <c r="B250" s="4"/>
+      <c r="B250" s="3"/>
     </row>
     <row r="251" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="2"/>
-      <c r="B251" s="4"/>
+      <c r="B251" s="3"/>
     </row>
     <row r="252" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="2"/>
-      <c r="B252" s="4"/>
+      <c r="B252" s="3"/>
     </row>
     <row r="253" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="2"/>
-      <c r="B253" s="4"/>
+      <c r="B253" s="3"/>
     </row>
     <row r="254" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" s="2"/>
-      <c r="B254" s="4"/>
+      <c r="B254" s="3"/>
     </row>
     <row r="255" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="2"/>
-      <c r="B255" s="4"/>
+      <c r="B255" s="3"/>
     </row>
     <row r="256" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="2"/>
-      <c r="B256" s="4"/>
+      <c r="B256" s="3"/>
     </row>
     <row r="257" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="2"/>
-      <c r="B257" s="4"/>
+      <c r="B257" s="3"/>
     </row>
     <row r="258" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="2"/>
-      <c r="B258" s="4"/>
+      <c r="B258" s="3"/>
     </row>
     <row r="259" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="2"/>
-      <c r="B259" s="4"/>
+      <c r="B259" s="3"/>
     </row>
     <row r="260" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" s="2"/>
-      <c r="B260" s="4"/>
+      <c r="B260" s="3"/>
     </row>
     <row r="261" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" s="2"/>
-      <c r="B261" s="4"/>
+      <c r="B261" s="3"/>
     </row>
     <row r="262" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" s="2"/>
-      <c r="B262" s="4"/>
+      <c r="B262" s="3"/>
     </row>
     <row r="263" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" s="2"/>
-      <c r="B263" s="4"/>
+      <c r="B263" s="3"/>
     </row>
     <row r="264" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" s="2"/>
-      <c r="B264" s="4"/>
+      <c r="B264" s="3"/>
     </row>
     <row r="265" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A265" s="2"/>
-      <c r="B265" s="4"/>
+      <c r="B265" s="3"/>
     </row>
     <row r="266" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" s="2"/>
-      <c r="B266" s="4"/>
+      <c r="B266" s="3"/>
     </row>
     <row r="267" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" s="2"/>
-      <c r="B267" s="4"/>
+      <c r="B267" s="3"/>
     </row>
     <row r="268" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" s="2"/>
-      <c r="B268" s="4"/>
+      <c r="B268" s="3"/>
     </row>
     <row r="269" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" s="2"/>
-      <c r="B269" s="4"/>
+      <c r="B269" s="3"/>
     </row>
     <row r="270" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" s="2"/>
-      <c r="B270" s="4"/>
+      <c r="B270" s="3"/>
     </row>
     <row r="271" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="272" spans="1:2" ht="21.2" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3522,5 +3502,6 @@
     <mergeCell ref="A167:B167"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>